<commit_message>
ReSplice Core 수정 $
#859
</commit_message>
<xml_diff>
--- a/Data/ReSplice Core - 3236303965/3236303965.xlsx
+++ b/Data/ReSplice Core - 3236303965/3236303965.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\Steam\steamapps\common\RimWorld\Mods\RMK\Data\ReSplice Core - 3236303965\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{782446BC-FD2C-428B-A827-29D452918B3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E18CF90-53A4-4FAE-9831-889A89668C0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="793" uniqueCount="549">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="794" uniqueCount="550">
   <si>
     <t>Class+Node [(Identifier (Key)]</t>
   </si>
@@ -1639,9 +1639,6 @@
     <t>subject-&gt;어둠의 초월인자 추출</t>
   </si>
   <si>
-    <t>공허 접촉' 상태 추가</t>
-  </si>
-  <si>
     <t>This building can store an huge amount of genepacks and make them usable to create new xenogerms, when placed near a gene assembler. Large gene libraries can be made more space efficient with gene registers.\n\nWhen powered, gene registers prevent genepacks from deteriorating and will slowly repair deterioration.</t>
   </si>
   <si>
@@ -1685,6 +1682,14 @@
   </si>
   <si>
     <t>{PAWN_nameDef}(은)는 이미 어둠의 인자를 지녔기 때문에 {1}(을)를 주입할 수 없습니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>'공허 접촉' 상태 추가</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>대상은 공허의 깊숙한 곳을 보고 공허의 정수를 마셨습니다. 공허는 대상을 유전자 단위부터 변화시켰고 그 안에서 존재하며 행동을 인도하고 육체를 왜곡합니다. 바로 지금부터 영원히!</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -2046,8 +2051,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE2D6877-484B-49B0-81A6-14D26980CF1E}">
   <dimension ref="A1:F142"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F142" sqref="F142"/>
+    <sheetView tabSelected="1" topLeftCell="A104" workbookViewId="0">
+      <selection activeCell="F143" sqref="F143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -2095,7 +2100,7 @@
         <v>9</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
@@ -2129,7 +2134,7 @@
         <v>9</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
@@ -2163,7 +2168,7 @@
         <v>21</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
@@ -2214,41 +2219,41 @@
         <v>38</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>27</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>27</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.45">
@@ -2552,7 +2557,7 @@
         <v>85</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>534</v>
+        <v>548</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.45">
@@ -4701,10 +4706,10 @@
         <v>524</v>
       </c>
       <c r="E141" s="1" t="s">
+        <v>546</v>
+      </c>
+      <c r="F141" s="3" t="s">
         <v>547</v>
-      </c>
-      <c r="F141" s="3" t="s">
-        <v>548</v>
       </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.45">
@@ -4723,7 +4728,9 @@
       <c r="E142" s="1" t="s">
         <v>411</v>
       </c>
-      <c r="F142" s="3"/>
+      <c r="F142" s="3" t="s">
+        <v>549</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>